<commit_message>
Update LoginTestdata file and testng.xml file
</commit_message>
<xml_diff>
--- a/src/main/resources/LoginCredential.xlsx
+++ b/src/main/resources/LoginCredential.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1152" windowWidth="14376" windowHeight="3828"/>
+    <workbookView xWindow="0" yWindow="1155" windowWidth="14370" windowHeight="3825"/>
   </bookViews>
   <sheets>
     <sheet name="teststeps" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>password</t>
   </si>
@@ -30,12 +29,15 @@
   <si>
     <t>Rajani@1992</t>
   </si>
+  <si>
+    <t>Sr no</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,7 +173,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -206,7 +207,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,64 +382,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="19.77734375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upadting join meeting page and test
</commit_message>
<xml_diff>
--- a/src/main/resources/LoginCredential.xlsx
+++ b/src/main/resources/LoginCredential.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1152" windowWidth="22152" windowHeight="9396"/>
+    <workbookView xWindow="0" yWindow="1152" windowWidth="12816" windowHeight="3720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="teststeps" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="jmeetdata" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:M11"/>
 </workbook>
 </file>
 
@@ -391,7 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -450,7 +450,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>